<commit_message>
PHEV subsidy percentage corrected to pull CA values
</commit_message>
<xml_diff>
--- a/InputData/trans/BPHEVSP/BAU PHEV Subsidy Perc.xlsx
+++ b/InputData/trans/BPHEVSP/BAU PHEV Subsidy Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\State Models\eps-newyork\InputData\trans\BPHEVSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\State Models\eps-california\InputData\trans\BPHEVSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87F57D13-A26B-4F8A-996A-C5F7AC257EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAFAEEA-5D1D-4F47-9ED6-D8D192A48998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="23085" windowHeight="13305" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB5E61F-7942-4515-8229-A2210CA98666}">
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1452,7 +1452,7 @@
         <v>58</v>
       </c>
       <c r="B16" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>53</v>
@@ -1525,7 +1525,7 @@
         <v>61</v>
       </c>
       <c r="B18" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>53</v>
@@ -1941,31 +1941,31 @@
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C33" s="2">
         <f t="shared" ref="C33" si="1">SUMPRODUCT(D13:D26,$B$13:$B$26)/SUM($B$13:$B$26)</f>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ref="D33" si="2">SUMPRODUCT(E13:E26,$B$13:$B$26)/SUM($B$13:$B$26)</f>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" ref="E33" si="3">SUMPRODUCT(F13:F26,$B$13:$B$26)/SUM($B$13:$B$26)</f>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" ref="F33" si="4">SUMPRODUCT(G13:G26,$B$13:$B$26)/SUM($B$13:$B$26)</f>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" ref="G33:I33" si="5">SUMPRODUCT(H13:H26,$B$13:$B$26)/SUM($B$13:$B$26)</f>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="J33" s="2">
         <v>0</v>
@@ -2206,31 +2206,31 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2">
         <f>(A3+C33)*About!$B$33</f>
-        <v>7089.0804836407387</v>
+        <v>8863.301826628478</v>
       </c>
       <c r="D38" s="2">
         <f>(B3+D33)*About!$B$33</f>
-        <v>7096.2738526461635</v>
+        <v>8870.4951956339028</v>
       </c>
       <c r="E38" s="2">
         <f>(C3+E33)*About!$B$33</f>
-        <v>4060.6060287258383</v>
+        <v>5834.8273717135789</v>
       </c>
       <c r="F38" s="2">
         <f>(D3+F33)*About!$B$33</f>
-        <v>1866.417433175201</v>
+        <v>3640.6387761629412</v>
       </c>
       <c r="G38" s="2">
         <f>(E3+G33)*About!$B$33</f>
-        <v>1282.0199650437494</v>
+        <v>3056.2413080314896</v>
       </c>
       <c r="H38" s="2">
         <f>(F3+H33)*About!$B$33</f>
-        <v>864.64370703529585</v>
+        <v>2638.8650500230365</v>
       </c>
       <c r="I38" s="2">
         <f>(G3+I33)*About!$B$33</f>
-        <v>744.07885409868288</v>
+        <v>2518.3001970864234</v>
       </c>
       <c r="J38" s="2">
         <f>(H3+J33)*About!$B$33</f>
@@ -2630,31 +2630,31 @@
       <c r="B45" s="7"/>
       <c r="C45" s="7">
         <f>C38/B41</f>
-        <v>0.19218891947190639</v>
+        <v>0.24028904805694512</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" ref="D45:AG45" si="7">D38/C41</f>
-        <v>0.19006009729346662</v>
+        <v>0.23757921621003034</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="7"/>
-        <v>0.10877885902986521</v>
+        <v>0.15630816179682228</v>
       </c>
       <c r="F45" s="7">
         <f t="shared" si="7"/>
-        <v>4.976715017932435E-2</v>
+        <v>9.7075934622908602E-2</v>
       </c>
       <c r="G45" s="7">
         <f t="shared" si="7"/>
-        <v>3.4168975614172425E-2</v>
+        <v>8.1456324840924563E-2</v>
       </c>
       <c r="H45" s="7">
         <f t="shared" si="7"/>
-        <v>2.2975067944818406E-2</v>
+        <v>7.011917548023161E-2</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="7"/>
-        <v>1.9751509187159771E-2</v>
+        <v>6.6848062143937764E-2</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="7"/>
@@ -15262,7 +15262,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AG15:AI24 AG3:AG14 B3:AF24">
+  <conditionalFormatting sqref="AG3:AG14 B3:AF24 AG15:AI24">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>B3&gt;600000</formula>
     </cfRule>
@@ -18746,31 +18746,31 @@
       </c>
       <c r="B2" s="9">
         <f>Summary!C38</f>
-        <v>7089.0804836407387</v>
+        <v>8863.301826628478</v>
       </c>
       <c r="C2" s="9">
         <f>Summary!D38</f>
-        <v>7096.2738526461635</v>
+        <v>8870.4951956339028</v>
       </c>
       <c r="D2" s="9">
         <f>Summary!E38</f>
-        <v>4060.6060287258383</v>
+        <v>5834.8273717135789</v>
       </c>
       <c r="E2" s="9">
         <f>Summary!F38</f>
-        <v>1866.417433175201</v>
+        <v>3640.6387761629412</v>
       </c>
       <c r="F2" s="9">
         <f>Summary!G38</f>
-        <v>1282.0199650437494</v>
+        <v>3056.2413080314896</v>
       </c>
       <c r="G2" s="9">
         <f>Summary!H38</f>
-        <v>864.64370703529585</v>
+        <v>2638.8650500230365</v>
       </c>
       <c r="H2" s="9">
         <f>Summary!I38</f>
-        <v>744.07885409868288</v>
+        <v>2518.3001970864234</v>
       </c>
       <c r="I2" s="9">
         <f>Summary!J38</f>

</xml_diff>